<commit_message>
double checked grain yields for SD 2023 and 2024 pre disposal
</commit_message>
<xml_diff>
--- a/data/Jl01_vcf_sample_name_to_accession_name.xlsx
+++ b/data/Jl01_vcf_sample_name_to_accession_name.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pth7\Documents\Intercrop JLJ\2024_spring\2024_spring\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAB72135-FA0C-487C-92F8-03D0F1BF5113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B869D2-84B8-48D4-96F3-F57E3CA6786C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30405" yWindow="0" windowWidth="20160" windowHeight="12360" xr2:uid="{5C70E7DB-6187-4C21-808B-327CF0D3E4D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5C70E7DB-6187-4C21-808B-327CF0D3E4D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1351,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B98C1E-7201-4AAE-8C91-BA8EA0C68FEB}">
   <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="H90" sqref="H90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>